<commit_message>
verify GPT prompt result
</commit_message>
<xml_diff>
--- a/Report/Presentation.xlsx
+++ b/Report/Presentation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/4rr311/Documents/VectorA/KHTN/Nam4/HKII/Thesis/Brainstorming/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A486F12-0389-DC44-A6E6-4E1B842EC299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A676DF9-5DD5-F94E-ADD7-D800413D4EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19440" xr2:uid="{2BE182E7-5BBB-9A4F-865F-D068BDBECF9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>1.1. Đặt vấn đề + 1.2. Mục tiêu</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Script</t>
   </si>
 </sst>
 </file>
@@ -116,15 +119,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,19 +153,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,137 +512,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE5083C-8E0D-9146-9E67-E7CE7CB9F567}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="3" max="3" width="77" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="168.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <f>A2</f>
+        <v>1</v>
+      </c>
+      <c r="B19" s="9" t="str">
+        <f t="shared" ref="B19:C19" si="0">B2</f>
+        <v>V</v>
+      </c>
+      <c r="C19" s="9" t="str">
+        <f>C2</f>
+        <v>1.1. Đặt vấn đề + 1.2. Mục tiêu</v>
+      </c>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9" t="str">
+        <f t="shared" ref="B20:C20" si="1">B3</f>
+        <v>V</v>
+      </c>
+      <c r="C20" s="9" t="str">
+        <f>C3</f>
+        <v>1.3. Các bước tiếp cận + 1.4. Đóng góp</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>3</v>
+      </c>
+      <c r="B21" s="9" t="str">
+        <f t="shared" ref="B21:C21" si="2">B4</f>
+        <v>V</v>
+      </c>
+      <c r="C21" s="9" t="str">
+        <f>C4</f>
+        <v>2.1. Các nghiên cứu + 2.2. Dữ liệu</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>4</v>
+      </c>
+      <c r="B22" s="10" t="str">
+        <f t="shared" ref="B22:D22" si="3">B5</f>
+        <v>H</v>
+      </c>
+      <c r="C22" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>2.3. Cơ sở lý thuyết + 2.4. Mô hình ngôn ngữ lớn</v>
+      </c>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>5</v>
+      </c>
+      <c r="B23" s="10" t="str">
+        <f t="shared" ref="B23:D23" si="4">B6</f>
+        <v>H</v>
+      </c>
+      <c r="C23" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>3.1. Vấn đề chi tiết + 3.2. Tổng quan phương pháp</v>
+      </c>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>6</v>
+      </c>
+      <c r="B24" s="9" t="str">
+        <f t="shared" ref="B24:D24" si="5">B7</f>
+        <v>V</v>
+      </c>
+      <c r="C24" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>3.3. Chuẩn bị dữ liệu</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>7</v>
+      </c>
+      <c r="B25" s="10" t="str">
+        <f t="shared" ref="B25:D25" si="6">B8</f>
+        <v>H</v>
+      </c>
+      <c r="C25" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>3.4. Kiến trúc mô hình + 3.5. text2att + 3.6. GPT2 LoRA + 3.7. Fairseq</v>
+      </c>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>8</v>
+      </c>
+      <c r="B26" s="9" t="str">
+        <f t="shared" ref="B26:C26" si="7">B9</f>
+        <v>V</v>
+      </c>
+      <c r="C26" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v>3.8. Hậu xử lý</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9" t="str">
+        <f t="shared" ref="B27:C27" si="8">B10</f>
+        <v>V</v>
+      </c>
+      <c r="C27" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v>3.9. Đánh giá mô hình</v>
+      </c>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>10</v>
+      </c>
+      <c r="B28" s="10" t="str">
+        <f t="shared" ref="B28:D28" si="9">B11</f>
+        <v>H</v>
+      </c>
+      <c r="C28" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v>4.1. Kết quả huấn luyện</v>
+      </c>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>11</v>
+      </c>
+      <c r="B29" s="10" t="str">
+        <f t="shared" ref="B29:D30" si="10">B12</f>
+        <v>H</v>
+      </c>
+      <c r="C29" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>4.2. Phần mềm demo</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>12</v>
+      </c>
+      <c r="B30" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>H</v>
+      </c>
+      <c r="C30" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>5. Kết luận</v>
+      </c>
+      <c r="D30" s="10"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B18 B31:B1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>